<commit_message>
Actualizacion de filtros proyecto-suma, cambio modelos relacionados a mb y cambio estilos bootstrap
</commit_message>
<xml_diff>
--- a/uploads/GestionPermisos/GestionPermisos_CambioLinea.xlsx
+++ b/uploads/GestionPermisos/GestionPermisos_CambioLinea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/GestionPermisos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_21DD22F9F613C8D6CA77484A00B5D95074521B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73EDA425-7743-4ADD-B08B-208E972EDE6E}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_21DD22F9F613C8D6CA77484A00B5D95074521B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0C978CD-B21B-4B5F-B44F-D2B33B2051BC}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>id_categoria</t>
   </si>
@@ -87,13 +87,16 @@
   </si>
   <si>
     <t>nan</t>
+  </si>
+  <si>
+    <t>total_clp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,16 +112,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -141,16 +164,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,7 +505,7 @@
     <col min="2" max="2" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +527,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -509,10 +551,13 @@
         <v>16</v>
       </c>
       <c r="G2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>15962400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -532,10 +577,13 @@
         <v>16</v>
       </c>
       <c r="G3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>14366160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -555,10 +603,13 @@
         <v>17</v>
       </c>
       <c r="G4" s="2">
-        <v>52.960999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4">
+        <v>11447849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -578,10 +629,13 @@
         <v>17</v>
       </c>
       <c r="G5" s="2">
-        <v>52.960999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5724294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -601,10 +655,13 @@
         <v>17</v>
       </c>
       <c r="G6" s="2">
-        <v>52.960999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -624,10 +681,13 @@
         <v>17</v>
       </c>
       <c r="G7" s="2">
-        <v>52.960999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5">
+        <v>10567700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -647,10 +707,13 @@
         <v>17</v>
       </c>
       <c r="G8" s="2">
-        <v>52.960999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5283850</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -670,7 +733,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="2">
-        <v>52.960999999999999</v>
+        <v>6</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5283850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>